<commit_message>
Updating Project well locations
</commit_message>
<xml_diff>
--- a/FInal_Project/NoFlow_Boundaries.xlsx
+++ b/FInal_Project/NoFlow_Boundaries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laura/Documents/Teaching/Groundwater_Modeling/HWRS582_Spring20/Course_Mat_Git/FInal_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB07EDC-37C5-8E44-9F0E-9466FD6C2E52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4F1F69-1186-E14A-93DC-AEEC3AF74332}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27900" yWindow="460" windowWidth="29900" windowHeight="28040" xr2:uid="{76ED07CC-4216-B149-B9A3-8A78C10F09A5}"/>
+    <workbookView xWindow="21300" yWindow="460" windowWidth="29900" windowHeight="28040" xr2:uid="{76ED07CC-4216-B149-B9A3-8A78C10F09A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Row</t>
   </si>
@@ -49,6 +49,27 @@
   <si>
     <t xml:space="preserve">Cells that are no flow in the bottom layer only </t>
   </si>
+  <si>
+    <t>Flow py index</t>
+  </si>
+  <si>
+    <t>Flopy idex</t>
+  </si>
+  <si>
+    <t>Aq</t>
+  </si>
+  <si>
+    <t>Ag</t>
+  </si>
+  <si>
+    <t>m1</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>Wells (Ag= agricultural well, Aq=town well, m1=monitoring well1, m2=monitoring well2)</t>
+  </si>
 </sst>
 </file>
 
@@ -63,7 +84,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -91,6 +112,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -242,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -259,6 +286,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,301 +602,407 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD7613CA-5890-FD4E-9AAB-B1452D4EB631}">
-  <dimension ref="A1:AY57"/>
+  <dimension ref="A2:BA61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="51" width="3.5" customWidth="1"/>
+    <col min="3" max="52" width="3.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:51" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>6</v>
+      </c>
+      <c r="J2">
+        <v>7</v>
+      </c>
+      <c r="K2">
+        <v>8</v>
+      </c>
+      <c r="L2">
+        <v>9</v>
+      </c>
+      <c r="M2">
+        <v>10</v>
+      </c>
+      <c r="N2">
+        <v>11</v>
+      </c>
+      <c r="O2">
+        <v>12</v>
+      </c>
+      <c r="P2">
+        <v>13</v>
+      </c>
+      <c r="Q2">
+        <v>14</v>
+      </c>
+      <c r="R2">
+        <v>15</v>
+      </c>
+      <c r="S2">
+        <v>16</v>
+      </c>
+      <c r="T2">
+        <v>17</v>
+      </c>
+      <c r="U2">
+        <v>18</v>
+      </c>
+      <c r="V2">
+        <v>19</v>
+      </c>
+      <c r="W2">
+        <v>20</v>
+      </c>
+      <c r="X2">
+        <v>21</v>
+      </c>
+      <c r="Y2">
+        <v>22</v>
+      </c>
+      <c r="Z2">
+        <v>23</v>
+      </c>
+      <c r="AA2">
+        <v>24</v>
+      </c>
+      <c r="AB2">
+        <v>25</v>
+      </c>
+      <c r="AC2">
+        <v>26</v>
+      </c>
+      <c r="AD2">
+        <v>27</v>
+      </c>
+      <c r="AE2">
+        <v>28</v>
+      </c>
+      <c r="AF2">
+        <v>29</v>
+      </c>
+      <c r="AG2">
+        <v>30</v>
+      </c>
+      <c r="AH2">
+        <v>31</v>
+      </c>
+      <c r="AI2">
+        <v>32</v>
+      </c>
+      <c r="AJ2">
+        <v>33</v>
+      </c>
+      <c r="AK2">
+        <v>34</v>
+      </c>
+      <c r="AL2">
+        <v>35</v>
+      </c>
+      <c r="AM2">
+        <v>36</v>
+      </c>
+      <c r="AN2">
+        <v>37</v>
+      </c>
+      <c r="AO2">
+        <v>38</v>
+      </c>
+      <c r="AP2">
+        <v>39</v>
+      </c>
+      <c r="AQ2">
+        <v>40</v>
+      </c>
+      <c r="AR2">
+        <v>41</v>
+      </c>
+      <c r="AS2">
+        <v>42</v>
+      </c>
+      <c r="AT2">
+        <v>43</v>
+      </c>
+      <c r="AU2">
+        <v>44</v>
+      </c>
+      <c r="AV2">
+        <v>45</v>
+      </c>
+      <c r="AW2">
+        <v>46</v>
+      </c>
+      <c r="AX2">
+        <v>47</v>
+      </c>
+      <c r="AY2">
+        <v>48</v>
+      </c>
+      <c r="AZ2">
+        <v>49</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:53" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="C3">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="E3">
         <v>3</v>
       </c>
-      <c r="E2">
+      <c r="F3">
         <v>4</v>
       </c>
-      <c r="F2">
+      <c r="G3">
         <v>5</v>
       </c>
-      <c r="G2">
+      <c r="H3">
         <v>6</v>
       </c>
-      <c r="H2">
+      <c r="I3">
         <v>7</v>
       </c>
-      <c r="I2">
+      <c r="J3">
         <v>8</v>
       </c>
-      <c r="J2">
+      <c r="K3">
         <v>9</v>
       </c>
-      <c r="K2">
+      <c r="L3">
         <v>10</v>
       </c>
-      <c r="L2">
+      <c r="M3">
         <v>11</v>
       </c>
-      <c r="M2">
+      <c r="N3">
         <v>12</v>
       </c>
-      <c r="N2">
+      <c r="O3">
         <v>13</v>
       </c>
-      <c r="O2">
+      <c r="P3">
         <v>14</v>
       </c>
-      <c r="P2">
+      <c r="Q3">
         <v>15</v>
       </c>
-      <c r="Q2">
+      <c r="R3">
         <v>16</v>
       </c>
-      <c r="R2">
+      <c r="S3">
         <v>17</v>
       </c>
-      <c r="S2">
+      <c r="T3">
         <v>18</v>
       </c>
-      <c r="T2">
+      <c r="U3">
         <v>19</v>
       </c>
-      <c r="U2">
+      <c r="V3">
         <v>20</v>
       </c>
-      <c r="V2">
+      <c r="W3">
         <v>21</v>
       </c>
-      <c r="W2">
+      <c r="X3">
         <v>22</v>
       </c>
-      <c r="X2">
+      <c r="Y3">
         <v>23</v>
       </c>
-      <c r="Y2">
+      <c r="Z3">
         <v>24</v>
       </c>
-      <c r="Z2">
+      <c r="AA3">
         <v>25</v>
       </c>
-      <c r="AA2">
+      <c r="AB3">
         <v>26</v>
       </c>
-      <c r="AB2">
+      <c r="AC3">
         <v>27</v>
       </c>
-      <c r="AC2">
+      <c r="AD3">
         <v>28</v>
       </c>
-      <c r="AD2">
+      <c r="AE3">
         <v>29</v>
       </c>
-      <c r="AE2">
+      <c r="AF3">
         <v>30</v>
       </c>
-      <c r="AF2">
+      <c r="AG3">
         <v>31</v>
       </c>
-      <c r="AG2">
+      <c r="AH3">
         <v>32</v>
       </c>
-      <c r="AH2">
+      <c r="AI3">
         <v>33</v>
       </c>
-      <c r="AI2">
+      <c r="AJ3">
         <v>34</v>
       </c>
-      <c r="AJ2">
+      <c r="AK3">
         <v>35</v>
       </c>
-      <c r="AK2">
+      <c r="AL3">
         <v>36</v>
       </c>
-      <c r="AL2">
+      <c r="AM3">
         <v>37</v>
       </c>
-      <c r="AM2">
+      <c r="AN3">
         <v>38</v>
       </c>
-      <c r="AN2">
+      <c r="AO3">
         <v>39</v>
       </c>
-      <c r="AO2">
+      <c r="AP3">
         <v>40</v>
       </c>
-      <c r="AP2">
+      <c r="AQ3">
         <v>41</v>
       </c>
-      <c r="AQ2">
+      <c r="AR3">
         <v>42</v>
       </c>
-      <c r="AR2">
+      <c r="AS3">
         <v>43</v>
       </c>
-      <c r="AS2">
+      <c r="AT3">
         <v>44</v>
       </c>
-      <c r="AT2">
+      <c r="AU3">
         <v>45</v>
       </c>
-      <c r="AU2">
+      <c r="AV3">
         <v>46</v>
       </c>
-      <c r="AV2">
+      <c r="AW3">
         <v>47</v>
       </c>
-      <c r="AW2">
+      <c r="AX3">
         <v>48</v>
       </c>
-      <c r="AX2">
+      <c r="AY3">
         <v>49</v>
       </c>
-      <c r="AY2">
+      <c r="AZ3">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="BA3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
         <v>50</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="10"/>
-      <c r="AB3" s="10"/>
-      <c r="AC3" s="10"/>
-      <c r="AD3" s="10"/>
-      <c r="AE3" s="10"/>
-      <c r="AF3" s="10"/>
-      <c r="AG3" s="10"/>
-      <c r="AH3" s="10"/>
-      <c r="AI3" s="10"/>
-      <c r="AJ3" s="10"/>
-      <c r="AK3" s="10"/>
-      <c r="AL3" s="10"/>
-      <c r="AM3" s="10"/>
-      <c r="AN3" s="10"/>
-      <c r="AO3" s="10"/>
-      <c r="AP3" s="10"/>
-      <c r="AQ3" s="10"/>
-      <c r="AR3" s="10"/>
-      <c r="AS3" s="10"/>
-      <c r="AT3" s="10"/>
-      <c r="AU3" s="10"/>
-      <c r="AV3" s="10"/>
-      <c r="AW3" s="10"/>
-      <c r="AX3" s="10"/>
-      <c r="AY3" s="2"/>
-    </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="10"/>
+      <c r="AB4" s="10"/>
+      <c r="AC4" s="10"/>
+      <c r="AD4" s="10"/>
+      <c r="AE4" s="10"/>
+      <c r="AF4" s="10"/>
+      <c r="AG4" s="10"/>
+      <c r="AH4" s="10"/>
+      <c r="AI4" s="10"/>
+      <c r="AJ4" s="10"/>
+      <c r="AK4" s="10"/>
+      <c r="AL4" s="10"/>
+      <c r="AM4" s="10"/>
+      <c r="AN4" s="10"/>
+      <c r="AO4" s="10"/>
+      <c r="AP4" s="10"/>
+      <c r="AQ4" s="10"/>
+      <c r="AR4" s="10"/>
+      <c r="AS4" s="10"/>
+      <c r="AT4" s="10"/>
+      <c r="AU4" s="10"/>
+      <c r="AV4" s="10"/>
+      <c r="AW4" s="10"/>
+      <c r="AX4" s="10"/>
+      <c r="AY4" s="10"/>
+      <c r="AZ4" s="2"/>
+    </row>
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
         <v>49</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
-      <c r="AE4" s="1"/>
-      <c r="AF4" s="1"/>
-      <c r="AG4" s="1"/>
-      <c r="AH4" s="1"/>
-      <c r="AI4" s="1"/>
-      <c r="AJ4" s="1"/>
-      <c r="AK4" s="1"/>
-      <c r="AL4" s="1"/>
-      <c r="AM4" s="1"/>
-      <c r="AN4" s="1"/>
-      <c r="AO4" s="1"/>
-      <c r="AP4" s="1"/>
-      <c r="AQ4" s="1"/>
-      <c r="AR4" s="1"/>
-      <c r="AS4" s="1"/>
-      <c r="AT4" s="1"/>
-      <c r="AU4" s="1"/>
-      <c r="AV4" s="1"/>
-      <c r="AW4" s="1"/>
-      <c r="AX4" s="1"/>
-      <c r="AY4" s="3"/>
-    </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>48</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="7"/>
+      <c r="C5" s="5"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -907,21 +1042,24 @@
       <c r="AV5" s="1"/>
       <c r="AW5" s="1"/>
       <c r="AX5" s="1"/>
-      <c r="AY5" s="3"/>
-    </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY5" s="1"/>
+      <c r="AZ5" s="3"/>
+    </row>
+    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>47</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>48</v>
+      </c>
+      <c r="C6" s="5"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -962,20 +1100,23 @@
       <c r="AV6" s="1"/>
       <c r="AW6" s="1"/>
       <c r="AX6" s="1"/>
-      <c r="AY6" s="3"/>
-    </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY6" s="1"/>
+      <c r="AZ6" s="3"/>
+    </row>
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>46</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>47</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -1017,19 +1158,22 @@
       <c r="AV7" s="1"/>
       <c r="AW7" s="1"/>
       <c r="AX7" s="1"/>
-      <c r="AY7" s="3"/>
-    </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY7" s="1"/>
+      <c r="AZ7" s="3"/>
+    </row>
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>45</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>46</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -1072,18 +1216,21 @@
       <c r="AV8" s="1"/>
       <c r="AW8" s="1"/>
       <c r="AX8" s="1"/>
-      <c r="AY8" s="3"/>
-    </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY8" s="1"/>
+      <c r="AZ8" s="3"/>
+    </row>
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>44</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>45</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1127,17 +1274,20 @@
       <c r="AV9" s="1"/>
       <c r="AW9" s="1"/>
       <c r="AX9" s="1"/>
-      <c r="AY9" s="3"/>
-    </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY9" s="1"/>
+      <c r="AZ9" s="3"/>
+    </row>
+    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>43</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>44</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1182,16 +1332,19 @@
       <c r="AV10" s="1"/>
       <c r="AW10" s="1"/>
       <c r="AX10" s="1"/>
-      <c r="AY10" s="3"/>
-    </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY10" s="1"/>
+      <c r="AZ10" s="3"/>
+    </row>
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>42</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>43</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1237,15 +1390,18 @@
       <c r="AV11" s="1"/>
       <c r="AW11" s="1"/>
       <c r="AX11" s="1"/>
-      <c r="AY11" s="3"/>
-    </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY11" s="1"/>
+      <c r="AZ11" s="3"/>
+    </row>
+    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>41</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>42</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="12"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -1292,14 +1448,17 @@
       <c r="AV12" s="1"/>
       <c r="AW12" s="1"/>
       <c r="AX12" s="1"/>
-      <c r="AY12" s="3"/>
-    </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY12" s="1"/>
+      <c r="AZ12" s="3"/>
+    </row>
+    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>40</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>41</v>
+      </c>
+      <c r="C13" s="5"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1347,14 +1506,17 @@
       <c r="AV13" s="1"/>
       <c r="AW13" s="1"/>
       <c r="AX13" s="1"/>
-      <c r="AY13" s="3"/>
-    </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY13" s="1"/>
+      <c r="AZ13" s="3"/>
+    </row>
+    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>39</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>40</v>
+      </c>
+      <c r="C14" s="5"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -1402,14 +1564,17 @@
       <c r="AV14" s="1"/>
       <c r="AW14" s="1"/>
       <c r="AX14" s="1"/>
-      <c r="AY14" s="3"/>
-    </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY14" s="1"/>
+      <c r="AZ14" s="3"/>
+    </row>
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>38</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>39</v>
+      </c>
+      <c r="C15" s="5"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -1457,14 +1622,17 @@
       <c r="AV15" s="1"/>
       <c r="AW15" s="1"/>
       <c r="AX15" s="1"/>
-      <c r="AY15" s="3"/>
-    </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY15" s="1"/>
+      <c r="AZ15" s="3"/>
+    </row>
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>37</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>38</v>
+      </c>
+      <c r="C16" s="5"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1512,14 +1680,17 @@
       <c r="AV16" s="1"/>
       <c r="AW16" s="1"/>
       <c r="AX16" s="1"/>
-      <c r="AY16" s="3"/>
-    </row>
-    <row r="17" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY16" s="1"/>
+      <c r="AZ16" s="3"/>
+    </row>
+    <row r="17" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>36</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>37</v>
+      </c>
+      <c r="C17" s="5"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1567,14 +1738,17 @@
       <c r="AV17" s="1"/>
       <c r="AW17" s="1"/>
       <c r="AX17" s="1"/>
-      <c r="AY17" s="3"/>
-    </row>
-    <row r="18" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY17" s="1"/>
+      <c r="AZ17" s="3"/>
+    </row>
+    <row r="18" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>35</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>36</v>
+      </c>
+      <c r="C18" s="5"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -1622,14 +1796,17 @@
       <c r="AV18" s="1"/>
       <c r="AW18" s="1"/>
       <c r="AX18" s="1"/>
-      <c r="AY18" s="3"/>
-    </row>
-    <row r="19" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY18" s="1"/>
+      <c r="AZ18" s="3"/>
+    </row>
+    <row r="19" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>34</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>35</v>
+      </c>
+      <c r="C19" s="5"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -1677,14 +1854,17 @@
       <c r="AV19" s="1"/>
       <c r="AW19" s="1"/>
       <c r="AX19" s="1"/>
-      <c r="AY19" s="3"/>
-    </row>
-    <row r="20" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY19" s="1"/>
+      <c r="AZ19" s="3"/>
+    </row>
+    <row r="20" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>33</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <v>34</v>
+      </c>
+      <c r="C20" s="5"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -1732,14 +1912,17 @@
       <c r="AV20" s="1"/>
       <c r="AW20" s="1"/>
       <c r="AX20" s="1"/>
-      <c r="AY20" s="3"/>
-    </row>
-    <row r="21" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY20" s="1"/>
+      <c r="AZ20" s="3"/>
+    </row>
+    <row r="21" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>32</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>33</v>
+      </c>
+      <c r="C21" s="5"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -1787,14 +1970,17 @@
       <c r="AV21" s="1"/>
       <c r="AW21" s="1"/>
       <c r="AX21" s="1"/>
-      <c r="AY21" s="3"/>
-    </row>
-    <row r="22" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY21" s="1"/>
+      <c r="AZ21" s="3"/>
+    </row>
+    <row r="22" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>31</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>32</v>
+      </c>
+      <c r="C22" s="5"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -1842,14 +2028,17 @@
       <c r="AV22" s="1"/>
       <c r="AW22" s="1"/>
       <c r="AX22" s="1"/>
-      <c r="AY22" s="3"/>
-    </row>
-    <row r="23" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY22" s="1"/>
+      <c r="AZ22" s="3"/>
+    </row>
+    <row r="23" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>30</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="B23">
+        <v>31</v>
+      </c>
+      <c r="C23" s="5"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -1897,14 +2086,17 @@
       <c r="AV23" s="1"/>
       <c r="AW23" s="1"/>
       <c r="AX23" s="1"/>
-      <c r="AY23" s="3"/>
-    </row>
-    <row r="24" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY23" s="1"/>
+      <c r="AZ23" s="3"/>
+    </row>
+    <row r="24" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>29</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <v>30</v>
+      </c>
+      <c r="C24" s="5"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -1952,14 +2144,17 @@
       <c r="AV24" s="1"/>
       <c r="AW24" s="1"/>
       <c r="AX24" s="1"/>
-      <c r="AY24" s="3"/>
-    </row>
-    <row r="25" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY24" s="1"/>
+      <c r="AZ24" s="3"/>
+    </row>
+    <row r="25" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>28</v>
-      </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="B25">
+        <v>29</v>
+      </c>
+      <c r="C25" s="5"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -2007,14 +2202,17 @@
       <c r="AV25" s="1"/>
       <c r="AW25" s="1"/>
       <c r="AX25" s="1"/>
-      <c r="AY25" s="3"/>
-    </row>
-    <row r="26" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY25" s="1"/>
+      <c r="AZ25" s="3"/>
+    </row>
+    <row r="26" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>27</v>
-      </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="B26">
+        <v>28</v>
+      </c>
+      <c r="C26" s="5"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -2062,14 +2260,17 @@
       <c r="AV26" s="1"/>
       <c r="AW26" s="1"/>
       <c r="AX26" s="1"/>
-      <c r="AY26" s="3"/>
-    </row>
-    <row r="27" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY26" s="1"/>
+      <c r="AZ26" s="3"/>
+    </row>
+    <row r="27" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="B27">
+        <v>27</v>
+      </c>
+      <c r="C27" s="5"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -2117,14 +2318,17 @@
       <c r="AV27" s="1"/>
       <c r="AW27" s="1"/>
       <c r="AX27" s="1"/>
-      <c r="AY27" s="3"/>
-    </row>
-    <row r="28" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY27" s="1"/>
+      <c r="AZ27" s="3"/>
+    </row>
+    <row r="28" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>25</v>
-      </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="B28">
+        <v>26</v>
+      </c>
+      <c r="C28" s="5"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -2172,14 +2376,17 @@
       <c r="AV28" s="1"/>
       <c r="AW28" s="1"/>
       <c r="AX28" s="1"/>
-      <c r="AY28" s="3"/>
-    </row>
-    <row r="29" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY28" s="1"/>
+      <c r="AZ28" s="3"/>
+    </row>
+    <row r="29" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>24</v>
-      </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="B29">
+        <v>25</v>
+      </c>
+      <c r="C29" s="5"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -2203,7 +2410,9 @@
       <c r="X29" s="1"/>
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
-      <c r="AA29" s="1"/>
+      <c r="AA29" s="16" t="s">
+        <v>10</v>
+      </c>
       <c r="AB29" s="1"/>
       <c r="AC29" s="1"/>
       <c r="AD29" s="1"/>
@@ -2227,14 +2436,17 @@
       <c r="AV29" s="1"/>
       <c r="AW29" s="1"/>
       <c r="AX29" s="1"/>
-      <c r="AY29" s="3"/>
-    </row>
-    <row r="30" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY29" s="1"/>
+      <c r="AZ29" s="3"/>
+    </row>
+    <row r="30" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>23</v>
-      </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="B30">
+        <v>24</v>
+      </c>
+      <c r="C30" s="5"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -2282,14 +2494,17 @@
       <c r="AV30" s="1"/>
       <c r="AW30" s="1"/>
       <c r="AX30" s="1"/>
-      <c r="AY30" s="3"/>
-    </row>
-    <row r="31" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY30" s="1"/>
+      <c r="AZ30" s="3"/>
+    </row>
+    <row r="31" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>22</v>
-      </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="B31">
+        <v>23</v>
+      </c>
+      <c r="C31" s="5"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -2337,14 +2552,17 @@
       <c r="AV31" s="1"/>
       <c r="AW31" s="1"/>
       <c r="AX31" s="1"/>
-      <c r="AY31" s="3"/>
-    </row>
-    <row r="32" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY31" s="1"/>
+      <c r="AZ31" s="3"/>
+    </row>
+    <row r="32" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>21</v>
-      </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="B32">
+        <v>22</v>
+      </c>
+      <c r="C32" s="5"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -2392,14 +2610,17 @@
       <c r="AV32" s="1"/>
       <c r="AW32" s="1"/>
       <c r="AX32" s="1"/>
-      <c r="AY32" s="3"/>
-    </row>
-    <row r="33" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY32" s="1"/>
+      <c r="AZ32" s="3"/>
+    </row>
+    <row r="33" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>20</v>
-      </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="B33">
+        <v>21</v>
+      </c>
+      <c r="C33" s="5"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -2436,7 +2657,9 @@
       <c r="AK33" s="1"/>
       <c r="AL33" s="1"/>
       <c r="AM33" s="1"/>
-      <c r="AN33" s="1"/>
+      <c r="AN33" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="AO33" s="1"/>
       <c r="AP33" s="1"/>
       <c r="AQ33" s="1"/>
@@ -2447,14 +2670,17 @@
       <c r="AV33" s="1"/>
       <c r="AW33" s="1"/>
       <c r="AX33" s="1"/>
-      <c r="AY33" s="3"/>
-    </row>
-    <row r="34" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY33" s="1"/>
+      <c r="AZ33" s="3"/>
+    </row>
+    <row r="34" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>19</v>
-      </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="B34">
+        <v>20</v>
+      </c>
+      <c r="C34" s="5"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -2502,14 +2728,17 @@
       <c r="AV34" s="1"/>
       <c r="AW34" s="1"/>
       <c r="AX34" s="1"/>
-      <c r="AY34" s="3"/>
-    </row>
-    <row r="35" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY34" s="1"/>
+      <c r="AZ34" s="3"/>
+    </row>
+    <row r="35" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>18</v>
-      </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="B35">
+        <v>19</v>
+      </c>
+      <c r="C35" s="5"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -2557,14 +2786,17 @@
       <c r="AV35" s="1"/>
       <c r="AW35" s="1"/>
       <c r="AX35" s="1"/>
-      <c r="AY35" s="3"/>
-    </row>
-    <row r="36" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY35" s="1"/>
+      <c r="AZ35" s="3"/>
+    </row>
+    <row r="36" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>17</v>
-      </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="B36">
+        <v>18</v>
+      </c>
+      <c r="C36" s="5"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -2612,14 +2844,17 @@
       <c r="AV36" s="1"/>
       <c r="AW36" s="1"/>
       <c r="AX36" s="1"/>
-      <c r="AY36" s="3"/>
-    </row>
-    <row r="37" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY36" s="1"/>
+      <c r="AZ36" s="3"/>
+    </row>
+    <row r="37" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>16</v>
-      </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="B37">
+        <v>17</v>
+      </c>
+      <c r="C37" s="5"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -2667,14 +2902,17 @@
       <c r="AV37" s="1"/>
       <c r="AW37" s="1"/>
       <c r="AX37" s="1"/>
-      <c r="AY37" s="3"/>
-    </row>
-    <row r="38" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY37" s="1"/>
+      <c r="AZ37" s="3"/>
+    </row>
+    <row r="38" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>15</v>
-      </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="B38">
+        <v>16</v>
+      </c>
+      <c r="C38" s="5"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -2722,14 +2960,17 @@
       <c r="AV38" s="1"/>
       <c r="AW38" s="1"/>
       <c r="AX38" s="1"/>
-      <c r="AY38" s="3"/>
-    </row>
-    <row r="39" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY38" s="1"/>
+      <c r="AZ38" s="3"/>
+    </row>
+    <row r="39" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>14</v>
-      </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="B39">
+        <v>15</v>
+      </c>
+      <c r="C39" s="5"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -2777,14 +3018,17 @@
       <c r="AV39" s="1"/>
       <c r="AW39" s="1"/>
       <c r="AX39" s="1"/>
-      <c r="AY39" s="3"/>
-    </row>
-    <row r="40" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY39" s="1"/>
+      <c r="AZ39" s="3"/>
+    </row>
+    <row r="40" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>13</v>
-      </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="B40">
+        <v>14</v>
+      </c>
+      <c r="C40" s="5"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -2832,14 +3076,17 @@
       <c r="AV40" s="1"/>
       <c r="AW40" s="1"/>
       <c r="AX40" s="1"/>
-      <c r="AY40" s="3"/>
-    </row>
-    <row r="41" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY40" s="1"/>
+      <c r="AZ40" s="3"/>
+    </row>
+    <row r="41" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>12</v>
-      </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="1"/>
+        <v>37</v>
+      </c>
+      <c r="B41">
+        <v>13</v>
+      </c>
+      <c r="C41" s="5"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -2851,7 +3098,9 @@
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
+      <c r="O41" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
@@ -2887,14 +3136,17 @@
       <c r="AV41" s="1"/>
       <c r="AW41" s="1"/>
       <c r="AX41" s="1"/>
-      <c r="AY41" s="3"/>
-    </row>
-    <row r="42" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY41" s="1"/>
+      <c r="AZ41" s="3"/>
+    </row>
+    <row r="42" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>11</v>
-      </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="B42">
+        <v>12</v>
+      </c>
+      <c r="C42" s="5"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -2906,7 +3158,9 @@
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
-      <c r="O42" s="1"/>
+      <c r="O42" s="16" t="s">
+        <v>8</v>
+      </c>
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
@@ -2942,14 +3196,17 @@
       <c r="AV42" s="1"/>
       <c r="AW42" s="1"/>
       <c r="AX42" s="1"/>
-      <c r="AY42" s="3"/>
-    </row>
-    <row r="43" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY42" s="1"/>
+      <c r="AZ42" s="3"/>
+    </row>
+    <row r="43" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>10</v>
-      </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="B43">
+        <v>11</v>
+      </c>
+      <c r="C43" s="5"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -2997,14 +3254,17 @@
       <c r="AV43" s="1"/>
       <c r="AW43" s="1"/>
       <c r="AX43" s="1"/>
-      <c r="AY43" s="3"/>
-    </row>
-    <row r="44" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY43" s="1"/>
+      <c r="AZ43" s="3"/>
+    </row>
+    <row r="44" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>9</v>
-      </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="12"/>
+        <v>40</v>
+      </c>
+      <c r="B44">
+        <v>10</v>
+      </c>
+      <c r="C44" s="5"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -3052,14 +3312,17 @@
       <c r="AV44" s="1"/>
       <c r="AW44" s="1"/>
       <c r="AX44" s="1"/>
-      <c r="AY44" s="3"/>
-    </row>
-    <row r="45" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY44" s="1"/>
+      <c r="AZ44" s="3"/>
+    </row>
+    <row r="45" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>8</v>
-      </c>
-      <c r="B45" s="5"/>
-      <c r="C45" s="12"/>
+        <v>41</v>
+      </c>
+      <c r="B45">
+        <v>9</v>
+      </c>
+      <c r="C45" s="5"/>
       <c r="D45" s="12"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -3107,14 +3370,17 @@
       <c r="AV45" s="1"/>
       <c r="AW45" s="1"/>
       <c r="AX45" s="1"/>
-      <c r="AY45" s="3"/>
-    </row>
-    <row r="46" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY45" s="1"/>
+      <c r="AZ45" s="3"/>
+    </row>
+    <row r="46" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>7</v>
-      </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="11"/>
+        <v>42</v>
+      </c>
+      <c r="B46">
+        <v>8</v>
+      </c>
+      <c r="C46" s="5"/>
       <c r="D46" s="12"/>
       <c r="E46" s="12"/>
       <c r="F46" s="1"/>
@@ -3162,14 +3428,17 @@
       <c r="AV46" s="1"/>
       <c r="AW46" s="1"/>
       <c r="AX46" s="1"/>
-      <c r="AY46" s="3"/>
-    </row>
-    <row r="47" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY46" s="1"/>
+      <c r="AZ46" s="3"/>
+    </row>
+    <row r="47" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>6</v>
-      </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="11"/>
+        <v>43</v>
+      </c>
+      <c r="B47">
+        <v>7</v>
+      </c>
+      <c r="C47" s="5"/>
       <c r="D47" s="11"/>
       <c r="E47" s="12"/>
       <c r="F47" s="12"/>
@@ -3217,14 +3486,17 @@
       <c r="AV47" s="1"/>
       <c r="AW47" s="1"/>
       <c r="AX47" s="1"/>
-      <c r="AY47" s="3"/>
-    </row>
-    <row r="48" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY47" s="1"/>
+      <c r="AZ47" s="3"/>
+    </row>
+    <row r="48" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>5</v>
-      </c>
-      <c r="B48" s="5"/>
-      <c r="C48" s="7"/>
+        <v>44</v>
+      </c>
+      <c r="B48">
+        <v>6</v>
+      </c>
+      <c r="C48" s="5"/>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
       <c r="F48" s="12"/>
@@ -3272,14 +3544,17 @@
       <c r="AV48" s="1"/>
       <c r="AW48" s="1"/>
       <c r="AX48" s="1"/>
-      <c r="AY48" s="3"/>
-    </row>
-    <row r="49" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY48" s="1"/>
+      <c r="AZ48" s="3"/>
+    </row>
+    <row r="49" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>4</v>
-      </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="7"/>
+        <v>45</v>
+      </c>
+      <c r="B49">
+        <v>5</v>
+      </c>
+      <c r="C49" s="5"/>
       <c r="D49" s="7"/>
       <c r="E49" s="11"/>
       <c r="F49" s="11"/>
@@ -3327,14 +3602,17 @@
       <c r="AV49" s="1"/>
       <c r="AW49" s="1"/>
       <c r="AX49" s="1"/>
-      <c r="AY49" s="3"/>
-    </row>
-    <row r="50" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY49" s="1"/>
+      <c r="AZ49" s="3"/>
+    </row>
+    <row r="50" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>3</v>
-      </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="7"/>
+        <v>46</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50" s="5"/>
       <c r="D50" s="7"/>
       <c r="E50" s="7"/>
       <c r="F50" s="11"/>
@@ -3382,14 +3660,17 @@
       <c r="AV50" s="1"/>
       <c r="AW50" s="1"/>
       <c r="AX50" s="1"/>
-      <c r="AY50" s="3"/>
-    </row>
-    <row r="51" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AY50" s="1"/>
+      <c r="AZ50" s="3"/>
+    </row>
+    <row r="51" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>2</v>
-      </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="7"/>
+        <v>47</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="C51" s="5"/>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
@@ -3437,79 +3718,147 @@
       <c r="AV51" s="1"/>
       <c r="AW51" s="1"/>
       <c r="AX51" s="1"/>
-      <c r="AY51" s="3"/>
-    </row>
-    <row r="52" spans="1:51" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AY51" s="1"/>
+      <c r="AZ51" s="3"/>
+    </row>
+    <row r="52" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A52">
+        <v>48</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52" s="5"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="12"/>
+      <c r="K52" s="12"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="1"/>
+      <c r="S52" s="1"/>
+      <c r="T52" s="1"/>
+      <c r="U52" s="1"/>
+      <c r="V52" s="1"/>
+      <c r="W52" s="1"/>
+      <c r="X52" s="1"/>
+      <c r="Y52" s="1"/>
+      <c r="Z52" s="1"/>
+      <c r="AA52" s="1"/>
+      <c r="AB52" s="1"/>
+      <c r="AC52" s="1"/>
+      <c r="AD52" s="1"/>
+      <c r="AE52" s="1"/>
+      <c r="AF52" s="1"/>
+      <c r="AG52" s="1"/>
+      <c r="AH52" s="1"/>
+      <c r="AI52" s="1"/>
+      <c r="AJ52" s="1"/>
+      <c r="AK52" s="1"/>
+      <c r="AL52" s="1"/>
+      <c r="AM52" s="1"/>
+      <c r="AN52" s="1"/>
+      <c r="AO52" s="1"/>
+      <c r="AP52" s="1"/>
+      <c r="AQ52" s="1"/>
+      <c r="AR52" s="1"/>
+      <c r="AS52" s="1"/>
+      <c r="AT52" s="1"/>
+      <c r="AU52" s="1"/>
+      <c r="AV52" s="1"/>
+      <c r="AW52" s="1"/>
+      <c r="AX52" s="1"/>
+      <c r="AY52" s="1"/>
+      <c r="AZ52" s="3"/>
+    </row>
+    <row r="53" spans="1:52" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>49</v>
+      </c>
+      <c r="B53">
         <v>1</v>
       </c>
-      <c r="B52" s="6"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
-      <c r="F52" s="8"/>
-      <c r="G52" s="8"/>
-      <c r="H52" s="8"/>
-      <c r="I52" s="8"/>
-      <c r="J52" s="8"/>
-      <c r="K52" s="8"/>
-      <c r="L52" s="8"/>
-      <c r="M52" s="8"/>
-      <c r="N52" s="8"/>
-      <c r="O52" s="8"/>
-      <c r="P52" s="8"/>
-      <c r="Q52" s="8"/>
-      <c r="R52" s="8"/>
-      <c r="S52" s="8"/>
-      <c r="T52" s="8"/>
-      <c r="U52" s="8"/>
-      <c r="V52" s="8"/>
-      <c r="W52" s="8"/>
-      <c r="X52" s="8"/>
-      <c r="Y52" s="8"/>
-      <c r="Z52" s="8"/>
-      <c r="AA52" s="8"/>
-      <c r="AB52" s="8"/>
-      <c r="AC52" s="8"/>
-      <c r="AD52" s="8"/>
-      <c r="AE52" s="8"/>
-      <c r="AF52" s="8"/>
-      <c r="AG52" s="8"/>
-      <c r="AH52" s="8"/>
-      <c r="AI52" s="8"/>
-      <c r="AJ52" s="8"/>
-      <c r="AK52" s="8"/>
-      <c r="AL52" s="8"/>
-      <c r="AM52" s="8"/>
-      <c r="AN52" s="8"/>
-      <c r="AO52" s="8"/>
-      <c r="AP52" s="8"/>
-      <c r="AQ52" s="8"/>
-      <c r="AR52" s="8"/>
-      <c r="AS52" s="8"/>
-      <c r="AT52" s="8"/>
-      <c r="AU52" s="8"/>
-      <c r="AV52" s="8"/>
-      <c r="AW52" s="8"/>
-      <c r="AX52" s="8"/>
-      <c r="AY52" s="4"/>
-    </row>
-    <row r="55" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="B55" s="14"/>
-      <c r="C55" t="s">
+      <c r="C53" s="6"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="8"/>
+      <c r="K53" s="8"/>
+      <c r="L53" s="8"/>
+      <c r="M53" s="8"/>
+      <c r="N53" s="8"/>
+      <c r="O53" s="8"/>
+      <c r="P53" s="8"/>
+      <c r="Q53" s="8"/>
+      <c r="R53" s="8"/>
+      <c r="S53" s="8"/>
+      <c r="T53" s="8"/>
+      <c r="U53" s="8"/>
+      <c r="V53" s="8"/>
+      <c r="W53" s="8"/>
+      <c r="X53" s="8"/>
+      <c r="Y53" s="8"/>
+      <c r="Z53" s="8"/>
+      <c r="AA53" s="8"/>
+      <c r="AB53" s="8"/>
+      <c r="AC53" s="8"/>
+      <c r="AD53" s="8"/>
+      <c r="AE53" s="8"/>
+      <c r="AF53" s="8"/>
+      <c r="AG53" s="8"/>
+      <c r="AH53" s="8"/>
+      <c r="AI53" s="8"/>
+      <c r="AJ53" s="8"/>
+      <c r="AK53" s="8"/>
+      <c r="AL53" s="8"/>
+      <c r="AM53" s="8"/>
+      <c r="AN53" s="8"/>
+      <c r="AO53" s="8"/>
+      <c r="AP53" s="8"/>
+      <c r="AQ53" s="8"/>
+      <c r="AR53" s="8"/>
+      <c r="AS53" s="8"/>
+      <c r="AT53" s="8"/>
+      <c r="AU53" s="8"/>
+      <c r="AV53" s="8"/>
+      <c r="AW53" s="8"/>
+      <c r="AX53" s="8"/>
+      <c r="AY53" s="8"/>
+      <c r="AZ53" s="4"/>
+    </row>
+    <row r="56" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="C56" s="14"/>
+      <c r="D56" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="B56" s="15"/>
-      <c r="C56" t="s">
+    <row r="57" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="C57" s="15"/>
+      <c r="D57" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="B57" s="13"/>
-      <c r="C57" t="s">
+    <row r="58" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="C58" s="13"/>
+      <c r="D58" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="C61" s="17"/>
+      <c r="D61" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>